<commit_message>
add intertexts mor-mou based on van der stempel
</commit_message>
<xml_diff>
--- a/data/intertexts.xlsx
+++ b/data/intertexts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikekestemont/GitRepos/mdu/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9248D27F-E5A2-9747-B1E9-BF4EB4B85466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D07530-10FB-C242-8C08-79EAC7D0AAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EE8F2A7F-140C-9241-9DA1-451951B6B8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="378">
   <si>
     <t>ID</t>
   </si>
@@ -804,13 +804,379 @@
   </si>
   <si>
     <t>mor-ele-80</t>
+  </si>
+  <si>
+    <t>mor-mou-1</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1914</t>
+  </si>
+  <si>
+    <t>Riddere metter mouwen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die met pinen gespreken conde. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doe hi met pinen gespreken mochte </t>
+  </si>
+  <si>
+    <t>Sine wonden ende deden eten / Ende dede hem sijns leets daer vergeten</t>
+  </si>
+  <si>
+    <t>mor-mou-2</t>
+  </si>
+  <si>
+    <t>Ende begonste drinken ende eten / Ende sijns leets vele vergeten</t>
+  </si>
+  <si>
+    <t>mor-mou-3</t>
+  </si>
+  <si>
+    <t>mor-mou-4</t>
+  </si>
+  <si>
+    <t>mor-mou-6</t>
+  </si>
+  <si>
+    <t>mor-mou-7</t>
+  </si>
+  <si>
+    <t>mor-mou-8</t>
+  </si>
+  <si>
+    <t>mor-mou-9</t>
+  </si>
+  <si>
+    <t>mor-mou-10</t>
+  </si>
+  <si>
+    <t>mor-mou-11</t>
+  </si>
+  <si>
+    <t>mor-mou-12</t>
+  </si>
+  <si>
+    <t>mor-mou-13</t>
+  </si>
+  <si>
+    <t>mor-mou-14</t>
+  </si>
+  <si>
+    <t>mor-mou-15</t>
+  </si>
+  <si>
+    <t>mor-mou-16</t>
+  </si>
+  <si>
+    <t>mor-mou-17</t>
+  </si>
+  <si>
+    <t>mor-mou-18</t>
+  </si>
+  <si>
+    <t>Ende doen die dienst was gedaen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tirst dattie dinst was gedaen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doe hi achters van hem sciet </t>
+  </si>
+  <si>
+    <t>Double case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doe hi achters van u sciet </t>
+  </si>
+  <si>
+    <t>Jonckbloet has spreken vs gespreken. Very similar case: "met pine te worde"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doe hi achterst van hare sciet </t>
+  </si>
+  <si>
+    <t>Already encountered</t>
+  </si>
+  <si>
+    <t>Van algader sinen mesdaden, / Die hi ml dede, u comt te genaden.</t>
+  </si>
+  <si>
+    <t>Want is come u te genaden / Van allen min en mesdaden</t>
+  </si>
+  <si>
+    <t>Ende bringen bier tuwe hove / Dien gi priest van selken love.</t>
+  </si>
+  <si>
+    <t>Ic salve bringen hier te hove / Al waer hi noch van merren love</t>
+  </si>
+  <si>
+    <t>Ic sal u bat beraden</t>
+  </si>
+  <si>
+    <t>Ende sal breken dese onsede / Oftic salre om sterven.</t>
+  </si>
+  <si>
+    <t>Ic wille ... u onsede / Vellen ... oftic sterve</t>
+  </si>
+  <si>
+    <t>Si reden te gadere beide nu / So sere dat haer speren braken : / Men horetse harde verre craken.</t>
+  </si>
+  <si>
+    <t>Ende quamen te samen met selken nide / Dat harde beider speren braken : / Men mochse verre horen craken.</t>
+  </si>
+  <si>
+    <t>Ontoet ! laet in !</t>
+  </si>
+  <si>
+    <t>Ontoet, laet in !</t>
+  </si>
+  <si>
+    <t>.. in dier gebare / Oft . . ware.</t>
+  </si>
+  <si>
+    <t>.. in din gebare / Alse oft . . ware</t>
+  </si>
+  <si>
+    <t>.. die ongemate / Was, gegaen metten drossate.</t>
+  </si>
+  <si>
+    <t>.. drossate, / Die fel was ende ongemate.</t>
+  </si>
+  <si>
+    <t>„Riddere, hoe comt datgi sijt / Dus haestech op genen tijt ?"</t>
+  </si>
+  <si>
+    <t>.. „Ens noch niet tijt; / Hoe komt dat gi dus haestech sijt?'</t>
+  </si>
+  <si>
+    <t>.. dor die scame / Om dat hi hadde ridders name</t>
+  </si>
+  <si>
+    <t>En ware dat hen ware scame / Omdat hi hadde ridders name.</t>
+  </si>
+  <si>
+    <t>.. Dore die noet / Moesten si gaen in enen boet.</t>
+  </si>
+  <si>
+    <t>Diene name in sinen boet .. / Dus moesti keren dor die noet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ende dadense also achtergaen. </t>
+  </si>
+  <si>
+    <t>Hie deetse bat achtergaen.</t>
+  </si>
+  <si>
+    <t>Editions have achterstaen. Might not be a link.</t>
+  </si>
+  <si>
+    <t>Hi sloechse neder bi .II., bi drien.</t>
+  </si>
+  <si>
+    <t>mor-mou-19</t>
+  </si>
+  <si>
+    <t>mor-mou-20</t>
+  </si>
+  <si>
+    <t>mor-mou-21</t>
+  </si>
+  <si>
+    <t>mor-mou-22</t>
+  </si>
+  <si>
+    <t>mor-mou-23</t>
+  </si>
+  <si>
+    <t>mor-mou-24</t>
+  </si>
+  <si>
+    <t>mor-mou-25</t>
+  </si>
+  <si>
+    <t>mor-mou-26</t>
+  </si>
+  <si>
+    <t>mor-mou-27</t>
+  </si>
+  <si>
+    <t>mor-mou-28</t>
+  </si>
+  <si>
+    <t>mor-mou-29</t>
+  </si>
+  <si>
+    <t>Ontwee oft ware een vilt.</t>
+  </si>
+  <si>
+    <t>Hi sloecht ontwee asst ware .I. riet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.. ende haer gewaden : / Dus waren si alle omberaden. </t>
+  </si>
+  <si>
+    <t>. ende sine gewaden / Waren harde omberaden.</t>
+  </si>
+  <si>
+    <t>. bi hem soude niet sijn tebroken / (: gesproken)</t>
+  </si>
+  <si>
+    <t>Ne werd si nembermeer tebroken / (: gesproken)</t>
+  </si>
+  <si>
+    <t>Ende die riddere en liet achter niet / Van dat hi . . behiet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hine wilde achterlaten niet Dat .. behiet. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sijn lybaerd scoretse toten voten. </t>
+  </si>
+  <si>
+    <t>Ende scordene toten voten daernaer</t>
+  </si>
+  <si>
+    <t>.. den casteel / Die van grauwen stene was opgewrocht.</t>
+  </si>
+  <si>
+    <t>Die casteel was wel gewrocht / Uten gronde van grauwen stene.</t>
+  </si>
+  <si>
+    <t>Doen dochte hen alien dbeste / Dat sine groven binnen harre veste.</t>
+  </si>
+  <si>
+    <t>Doen dochte Waleweine dbeste / Dat si voren binnen der veste.</t>
+  </si>
+  <si>
+    <t>souden sire licgen .VII. jaer.</t>
+  </si>
+  <si>
+    <t>Al soudire .VII. jaer licgen vore</t>
+  </si>
+  <si>
+    <t>Dat hi ware der bester een / Die den sonne nie besceen</t>
+  </si>
+  <si>
+    <t>.. die beste riddere een / Die de sonne nie besceen.</t>
+  </si>
+  <si>
+    <t>Si hadden gode orsse bescreden / (: gereden)</t>
+  </si>
+  <si>
+    <t>Ende hadde starke orsse bescreden / (: gereden)</t>
+  </si>
+  <si>
+    <t>Dattie coninc van Yrlant / Selve moeste gaen in hant / Ende liet hem den riddere vaen: / Doe was dat striden scire gedaen.</t>
+  </si>
+  <si>
+    <t>Alse die bataelge was gedaen / Si hadden voles vele gevaen / Ende den coninc van Yrlant: / Het was hen wel gegaen in hant.</t>
+  </si>
+  <si>
+    <t>Perchevael ende min her Walewein / Daden wonder in dat playn.</t>
+  </si>
+  <si>
+    <t>Ende van Perchevale, die opten pleine / Menegen brachten in anxte groet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soe waent u bat beraden. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi deetse vallen bi tween, bi drien. </t>
+  </si>
+  <si>
+    <t>Van der Stempel 1915</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1916</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1917</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1918</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1919</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1920</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1921</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1922</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1923</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1924</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1925</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1926</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1927</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1928</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1929</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1930</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1931</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1932</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1933</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1934</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1935</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1936</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1937</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1938</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1939</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1940</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1941</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1942</t>
+  </si>
+  <si>
+    <t>Van der Stempel 1943</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -823,12 +1189,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -864,18 +1224,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1192,1981 +1546,2612 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877CE539-07AB-BA4D-9F84-757ABF310EC0}">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="41" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="1"/>
-    <col min="7" max="7" width="15" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="23" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="33.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="41" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="15" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4">
-        <v>1</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="4">
-        <v>2</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="4">
-        <v>1</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="4">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <v>3</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="G6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="4">
-        <v>1</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="4">
-        <v>2</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="F9" s="2">
+        <v>2</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="4">
-        <v>1</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="4">
-        <v>2</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="F11" s="2">
+        <v>2</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="4">
-        <v>2</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="F12" s="2">
+        <v>2</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="4">
-        <v>1</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="4">
-        <v>1</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="4">
-        <v>1</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="4">
-        <v>2</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="F16" s="2">
+        <v>2</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="4">
-        <v>2</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="F17" s="2">
+        <v>2</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="4">
-        <v>2</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="F18" s="2">
+        <v>2</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="4">
-        <v>1</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F20" s="4">
-        <v>2</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="F20" s="2">
+        <v>2</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="4">
-        <v>2</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="F21" s="2">
+        <v>2</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="4">
-        <v>2</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="F22" s="2">
+        <v>2</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F23" s="4">
-        <v>2</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="F23" s="2">
+        <v>2</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F24" s="4">
-        <v>2</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+      <c r="F24" s="2">
+        <v>2</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F25" s="4">
-        <v>1</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F26" s="4">
-        <v>2</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="F26" s="2">
+        <v>2</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="B27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F27" s="4">
-        <v>1</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+      <c r="F27" s="2">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F28" s="4">
-        <v>1</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H28" s="4"/>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F29" s="4">
-        <v>1</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="4" t="s">
+      <c r="F29" s="2">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F30" s="4">
-        <v>1</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+      <c r="F30" s="2">
+        <v>1</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F31" s="4">
-        <v>1</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+      <c r="F31" s="2">
+        <v>1</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32" s="2">
         <v>3</v>
       </c>
-      <c r="G32" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+      <c r="G32" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F33" s="4">
-        <v>1</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+      <c r="F33" s="2">
+        <v>1</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F34" s="4">
-        <v>2</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+      <c r="F34" s="2">
+        <v>2</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="4" t="s">
+      <c r="B35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F35" s="4">
-        <v>1</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+      <c r="F35" s="2">
+        <v>1</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F36" s="4">
-        <v>1</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+      <c r="F36" s="2">
+        <v>1</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F37" s="4">
-        <v>2</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+      <c r="F37" s="2">
+        <v>2</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F38" s="4">
-        <v>1</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+      <c r="F38" s="2">
+        <v>1</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F39" s="4">
-        <v>2</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+      <c r="F39" s="2">
+        <v>2</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F40" s="4">
-        <v>2</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H40" s="4" t="s">
+      <c r="F40" s="2">
+        <v>2</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+    <row r="41" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F41" s="4">
-        <v>1</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H41" s="4"/>
-    </row>
-    <row r="42" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
+      <c r="F41" s="2">
+        <v>1</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F42" s="4">
-        <v>2</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H42" s="4"/>
-    </row>
-    <row r="43" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
+      <c r="F42" s="2">
+        <v>2</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C43" s="4" t="s">
+      <c r="B43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="F43" s="4">
-        <v>2</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H43" s="4"/>
-    </row>
-    <row r="44" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
+      <c r="F43" s="2">
+        <v>2</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="F44" s="4">
-        <v>1</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H44" s="4"/>
-    </row>
-    <row r="45" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+      <c r="F44" s="2">
+        <v>1</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F45" s="4">
-        <v>2</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H45" s="4"/>
-    </row>
-    <row r="46" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+      <c r="F45" s="2">
+        <v>2</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="F46" s="4">
-        <v>2</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H46" s="4"/>
-    </row>
-    <row r="47" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+      <c r="F46" s="2">
+        <v>2</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F47" s="4">
-        <v>1</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H47" s="4"/>
-    </row>
-    <row r="48" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
+      <c r="F47" s="2">
+        <v>1</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F48" s="4">
-        <v>1</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H48" s="4"/>
-    </row>
-    <row r="49" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
+      <c r="F48" s="2">
+        <v>1</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F49" s="4">
-        <v>1</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H49" s="4"/>
-    </row>
-    <row r="50" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
+      <c r="F49" s="2">
+        <v>1</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F50" s="4">
+      <c r="F50" s="2">
         <v>3</v>
       </c>
-      <c r="G50" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H50" s="4"/>
-    </row>
-    <row r="51" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
+      <c r="G50" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F51" s="4">
-        <v>2</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H51" s="4"/>
-    </row>
-    <row r="52" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
+      <c r="F51" s="2">
+        <v>2</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F52" s="4">
-        <v>1</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H52" s="4"/>
+      <c r="F52" s="2">
+        <v>1</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="53" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="F53" s="4">
-        <v>1</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H53" s="4" t="s">
+      <c r="F53" s="2">
+        <v>1</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H53" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
+    <row r="54" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B54" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C54" s="4" t="s">
+      <c r="B54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F54" s="4">
-        <v>2</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H54" s="4"/>
-    </row>
-    <row r="55" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
+      <c r="F54" s="2">
+        <v>2</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F55" s="4">
-        <v>1</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H55" s="4"/>
-    </row>
-    <row r="56" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
+      <c r="F55" s="2">
+        <v>1</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="F56" s="4">
-        <v>2</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H56" s="4"/>
-    </row>
-    <row r="57" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A57" s="4" t="s">
+      <c r="F56" s="2">
+        <v>2</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="F57" s="4">
-        <v>1</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H57" s="4"/>
+      <c r="F57" s="2">
+        <v>1</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="58" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C58" s="4" t="s">
+      <c r="B58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="F58" s="4">
-        <v>1</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H58" s="4" t="s">
+      <c r="F58" s="2">
+        <v>1</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H58" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
+    <row r="59" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="F59" s="4">
-        <v>2</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H59" s="4" t="s">
+      <c r="F59" s="2">
+        <v>2</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H59" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
+    <row r="60" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D60" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F60" s="4">
-        <v>1</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H60" s="4"/>
-    </row>
-    <row r="61" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
+      <c r="F60" s="2">
+        <v>1</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="F61" s="4">
-        <v>2</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H61" s="4"/>
-    </row>
-    <row r="62" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
+      <c r="F61" s="2">
+        <v>2</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="F62" s="4">
-        <v>2</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H62" s="4"/>
-    </row>
-    <row r="63" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
+      <c r="F62" s="2">
+        <v>2</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D63" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="F63" s="4">
-        <v>2</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H63" s="4"/>
-    </row>
-    <row r="64" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
+      <c r="F63" s="2">
+        <v>2</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D64" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="F64" s="4">
-        <v>1</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H64" s="4"/>
-    </row>
-    <row r="65" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
+      <c r="F64" s="2">
+        <v>1</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="F65" s="4">
-        <v>2</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H65" s="4"/>
-    </row>
-    <row r="66" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
+      <c r="F65" s="2">
+        <v>2</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D66" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="F66" s="4">
-        <v>2</v>
-      </c>
-      <c r="G66" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H66" s="4"/>
-    </row>
-    <row r="67" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
+      <c r="F66" s="2">
+        <v>2</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="F67" s="4">
-        <v>2</v>
-      </c>
-      <c r="G67" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H67" s="4"/>
-    </row>
-    <row r="68" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
+      <c r="F67" s="2">
+        <v>2</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D68" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="F68" s="4">
-        <v>1</v>
-      </c>
-      <c r="G68" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H68" s="4"/>
-    </row>
-    <row r="69" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
+      <c r="F68" s="2">
+        <v>1</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D69" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="F69" s="4">
-        <v>2</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H69" s="4"/>
-    </row>
-    <row r="70" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
+      <c r="F69" s="2">
+        <v>2</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="D70" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="F70" s="4">
-        <v>2</v>
-      </c>
-      <c r="G70" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H70" s="4"/>
-    </row>
-    <row r="71" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
+      <c r="F70" s="2">
+        <v>2</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B71" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C71" s="4" t="s">
+      <c r="B71" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D71" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="F71" s="4">
-        <v>2</v>
-      </c>
-      <c r="G71" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H71" s="4"/>
-    </row>
-    <row r="72" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A72" s="4" t="s">
+      <c r="F71" s="2">
+        <v>2</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D72" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="F72" s="4">
-        <v>1</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H72" s="4"/>
-    </row>
-    <row r="73" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
+      <c r="F72" s="2">
+        <v>1</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B73" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C73" s="4" t="s">
+      <c r="B73" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="D73" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="F73" s="4">
+      <c r="F73" s="2">
         <v>3</v>
       </c>
-      <c r="G73" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H73" s="4"/>
-    </row>
-    <row r="74" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
+      <c r="G73" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D74" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="F74" s="4">
-        <v>1</v>
-      </c>
-      <c r="G74" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H74" s="4"/>
-    </row>
-    <row r="75" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
+      <c r="F74" s="2">
+        <v>1</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D75" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E75" s="4" t="s">
+      <c r="D75" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="F75" s="4">
-        <v>2</v>
-      </c>
-      <c r="G75" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H75" s="4"/>
-    </row>
-    <row r="76" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
+      <c r="F75" s="2">
+        <v>2</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="D76" s="4" t="s">
+      <c r="D76" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="F76" s="4">
-        <v>1</v>
-      </c>
-      <c r="G76" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H76" s="4" t="s">
+      <c r="F76" s="2">
+        <v>1</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H76" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
+    <row r="77" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="D77" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="F77" s="4">
-        <v>1</v>
-      </c>
-      <c r="G77" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H77" s="4"/>
-    </row>
-    <row r="78" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A78" s="4" t="s">
+      <c r="F77" s="2">
+        <v>1</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="D78" s="4" t="s">
+      <c r="D78" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="F78" s="4">
-        <v>1</v>
-      </c>
-      <c r="G78" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H78" s="4"/>
-    </row>
-    <row r="79" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A79" s="4" t="s">
+      <c r="F78" s="2">
+        <v>1</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="D79" s="4" t="s">
+      <c r="D79" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="F79" s="4">
-        <v>2</v>
-      </c>
-      <c r="G79" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H79" s="4"/>
-    </row>
-    <row r="80" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A80" s="4" t="s">
+      <c r="F79" s="2">
+        <v>2</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="D80" s="4" t="s">
+      <c r="D80" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="F80" s="4">
-        <v>2</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H80" s="4"/>
-    </row>
-    <row r="81" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A81" s="4" t="s">
+      <c r="F80" s="2">
+        <v>2</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="D81" s="4" t="s">
+      <c r="D81" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="F81" s="4">
-        <v>1</v>
-      </c>
-      <c r="G81" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H81" s="4"/>
+      <c r="F81" s="2">
+        <v>1</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="170" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F82" s="2">
+        <v>1</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="F83" s="2">
+        <v>2</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F84" s="2">
+        <v>1</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="F85" s="2">
+        <v>1</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="F86" s="2">
+        <v>1</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="F87" s="2">
+        <v>2</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="F88" s="2">
+        <v>2</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F89" s="2">
+        <v>1</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F90" s="2">
+        <v>2</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F91" s="2">
+        <v>3</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F92" s="2">
+        <v>1</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F93" s="2">
+        <v>2</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F94" s="2">
+        <v>2</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="F95" s="2">
+        <v>2</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F96" s="2">
+        <v>2</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="F97" s="2">
+        <v>2</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F98" s="2">
+        <v>1</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="I98" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F99" s="2">
+        <v>1</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F100" s="2">
+        <v>1</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="F101" s="2">
+        <v>2</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="F102" s="2">
+        <v>2</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="F103" s="2">
+        <v>2</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F104" s="2">
+        <v>1</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F105" s="2">
+        <v>2</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F106" s="2">
+        <v>2</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="F107" s="2">
+        <v>1</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F108" s="2">
+        <v>1</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="F109" s="2">
+        <v>2</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="F110" s="2">
+        <v>4</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="F111" s="2">
+        <v>2</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>377</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
allow multiple intertext case, also within same text
</commit_message>
<xml_diff>
--- a/data/intertexts.xlsx
+++ b/data/intertexts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikekestemont/GitRepos/mdu/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D07530-10FB-C242-8C08-79EAC7D0AAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B20C0A2-4117-BC4C-B834-18B811FDC4B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EE8F2A7F-140C-9241-9DA1-451951B6B8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="379">
   <si>
     <t>ID</t>
   </si>
@@ -629,9 +629,6 @@
     <t>Daer hi vant enen casteel Sijn herte was sonder riuiel.</t>
   </si>
   <si>
-    <t>Ignored third tripleton</t>
-  </si>
-  <si>
     <t>Hi hadde sijn wapen af ghedaen:</t>
   </si>
   <si>
@@ -1170,6 +1167,12 @@
   </si>
   <si>
     <t>Van der Stempel 1943</t>
+  </si>
+  <si>
+    <t>Double case, cf. next one</t>
+  </si>
+  <si>
+    <t>Dus waren si snachs inden casteel / Sonder spel ende enech riveel</t>
   </si>
 </sst>
 </file>
@@ -1546,10 +1549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877CE539-07AB-BA4D-9F84-757ABF310EC0}">
-  <dimension ref="A1:I111"/>
+  <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2921,7 +2924,7 @@
         <v>9</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>196</v>
+        <v>378</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>10</v>
@@ -2936,27 +2939,27 @@
         <v>7</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>197</v>
+        <v>377</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F60" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>7</v>
@@ -2964,22 +2967,22 @@
     </row>
     <row r="61" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F61" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>7</v>
@@ -2987,19 +2990,19 @@
     </row>
     <row r="62" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F62" s="2">
         <v>2</v>
@@ -3010,19 +3013,19 @@
     </row>
     <row r="63" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F63" s="2">
         <v>2</v>
@@ -3033,22 +3036,22 @@
     </row>
     <row r="64" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F64" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>7</v>
@@ -3056,22 +3059,22 @@
     </row>
     <row r="65" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F65" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>7</v>
@@ -3079,19 +3082,19 @@
     </row>
     <row r="66" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F66" s="2">
         <v>2</v>
@@ -3102,19 +3105,19 @@
     </row>
     <row r="67" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F67" s="2">
         <v>2</v>
@@ -3125,22 +3128,22 @@
     </row>
     <row r="68" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="F68" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>7</v>
@@ -3148,22 +3151,22 @@
     </row>
     <row r="69" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F69" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>7</v>
@@ -3171,19 +3174,19 @@
     </row>
     <row r="70" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F70" s="2">
         <v>2</v>
@@ -3194,19 +3197,19 @@
     </row>
     <row r="71" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F71" s="2">
         <v>2</v>
@@ -3217,22 +3220,22 @@
     </row>
     <row r="72" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F72" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>7</v>
@@ -3240,22 +3243,22 @@
     </row>
     <row r="73" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F73" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>7</v>
@@ -3263,22 +3266,22 @@
     </row>
     <row r="74" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="F74" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>7</v>
@@ -3286,22 +3289,22 @@
     </row>
     <row r="75" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F75" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>7</v>
@@ -3309,68 +3312,68 @@
     </row>
     <row r="76" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F76" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="H76" s="2" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F77" s="2">
         <v>1</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F78" s="2">
         <v>1</v>
@@ -3381,22 +3384,22 @@
     </row>
     <row r="79" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F79" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>7</v>
@@ -3404,19 +3407,19 @@
     </row>
     <row r="80" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F80" s="2">
         <v>2</v>
@@ -3427,730 +3430,753 @@
     </row>
     <row r="81" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F81" s="2">
+        <v>2</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F82" s="2">
+        <v>1</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="170" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="F81" s="2">
-        <v>1</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="170" x14ac:dyDescent="0.2">
-      <c r="A82" s="2" t="s">
+      <c r="B83" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F83" s="2">
+        <v>1</v>
+      </c>
+      <c r="G83" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="F82" s="2">
-        <v>1</v>
-      </c>
-      <c r="G82" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="I82" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A83" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="F83" s="2">
-        <v>2</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>349</v>
+      <c r="I83" s="2" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>279</v>
+        <v>260</v>
       </c>
       <c r="F84" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F85" s="2">
         <v>1</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>282</v>
+        <v>349</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C86" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F86" s="2">
+        <v>1</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F87" s="2">
+        <v>1</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F88" s="2">
+        <v>2</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="I88" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="F86" s="2">
-        <v>1</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="I86" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A87" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="F87" s="2">
-        <v>2</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="I87" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A88" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="F88" s="2">
-        <v>2</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>347</v>
+        <v>288</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F89" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="F90" s="2">
+        <v>1</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F91" s="2">
+        <v>2</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C90" s="2" t="s">
+      <c r="B92" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E92" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="D90" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="F90" s="2">
-        <v>2</v>
-      </c>
-      <c r="G90" s="2" t="s">
+      <c r="F92" s="2">
+        <v>3</v>
+      </c>
+      <c r="G92" s="2" t="s">
         <v>356</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A91" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F91" s="2">
-        <v>3</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A92" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="F92" s="2">
-        <v>1</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F93" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F94" s="2">
         <v>2</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F95" s="2">
         <v>2</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F96" s="2">
         <v>2</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="F97" s="2">
+        <v>2</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="F98" s="2">
+        <v>2</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B97" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C97" s="2" t="s">
+      <c r="B99" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E99" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="D97" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="F97" s="2">
-        <v>2</v>
-      </c>
-      <c r="G97" s="2" t="s">
+      <c r="F99" s="2">
+        <v>1</v>
+      </c>
+      <c r="G99" s="2" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A98" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C98" s="2" t="s">
+      <c r="I99" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="F98" s="2">
-        <v>1</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="I98" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A99" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="F99" s="2">
-        <v>1</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>324</v>
+        <v>347</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="F100" s="2">
         <v>1</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>312</v>
+        <v>277</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="F101" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F102" s="2">
         <v>2</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F103" s="2">
         <v>2</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F104" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="F105" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="F106" s="2">
         <v>2</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F107" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F108" s="2">
         <v>1</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="F109" s="2">
+        <v>1</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F110" s="2">
+        <v>2</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="B109" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C109" s="2" t="s">
+      <c r="B111" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E111" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="D109" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="F109" s="2">
-        <v>2</v>
-      </c>
-      <c r="G109" s="2" t="s">
+      <c r="F111" s="2">
+        <v>4</v>
+      </c>
+      <c r="G111" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A110" s="2" t="s">
+    <row r="112" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B110" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C110" s="2" t="s">
+      <c r="B112" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E112" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="D110" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E110" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="F110" s="2">
-        <v>4</v>
-      </c>
-      <c r="G110" s="2" t="s">
+      <c r="F112" s="2">
+        <v>2</v>
+      </c>
+      <c r="G112" s="2" t="s">
         <v>376</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A111" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="F111" s="2">
-        <v>2</v>
-      </c>
-      <c r="G111" s="2" t="s">
-        <v>377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
intertexts from Moriaen (II)
</commit_message>
<xml_diff>
--- a/data/intertexts.xlsx
+++ b/data/intertexts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikekestemont/GitRepos/mdu/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178A9769-4E0D-E742-9831-A86365180DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E405E48-672B-6946-9B53-6CDA2ABDC1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EE8F2A7F-140C-9241-9DA1-451951B6B8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="687">
   <si>
     <t>ID</t>
   </si>
@@ -2079,6 +2079,24 @@
   </si>
   <si>
     <t> mor-ele-34</t>
+  </si>
+  <si>
+    <t>Doe die dienst was gedaen:</t>
+  </si>
+  <si>
+    <t>Doe die dinst was gedaen.</t>
+  </si>
+  <si>
+    <t>lan-ele-75</t>
+  </si>
+  <si>
+    <t>lan-ele-76</t>
+  </si>
+  <si>
+    <t>Entie ridders allegader Badens der auenturen vader Waleweine:</t>
+  </si>
+  <si>
+    <t>Doen sagen si daer allegader Op waleweine der auenturen vader.</t>
   </si>
 </sst>
 </file>
@@ -2100,13 +2118,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2116,7 +2129,13 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
@@ -2469,52 +2488,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877CE539-07AB-BA4D-9F84-757ABF310EC0}">
-  <dimension ref="A1:I229"/>
+  <dimension ref="A1:I230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A224" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C214" sqref="C214"/>
+    <sheetView tabSelected="1" topLeftCell="A216" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C233" sqref="C233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23" style="3" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="33.1640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="41" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="3"/>
-    <col min="7" max="7" width="15" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="23" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="33.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="41" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="15" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2536,10 +2554,8 @@
       <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -2561,10 +2577,8 @@
       <c r="G3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -2586,10 +2600,8 @@
       <c r="G4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -2611,10 +2623,8 @@
       <c r="G5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -2636,10 +2646,8 @@
       <c r="G6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -2661,10 +2669,8 @@
       <c r="G7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -2686,10 +2692,8 @@
       <c r="G8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
@@ -2711,10 +2715,8 @@
       <c r="G9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
@@ -2736,10 +2738,8 @@
       <c r="G10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
@@ -2761,10 +2761,8 @@
       <c r="G11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
@@ -2786,10 +2784,8 @@
       <c r="G12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>45</v>
       </c>
@@ -2811,10 +2807,8 @@
       <c r="G13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>48</v>
       </c>
@@ -2836,10 +2830,8 @@
       <c r="G14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
@@ -2861,10 +2853,8 @@
       <c r="G15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>54</v>
       </c>
@@ -2886,10 +2876,8 @@
       <c r="G16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>57</v>
       </c>
@@ -2911,10 +2899,8 @@
       <c r="G17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>60</v>
       </c>
@@ -2936,10 +2922,8 @@
       <c r="G18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>63</v>
       </c>
@@ -2961,10 +2945,8 @@
       <c r="G19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>66</v>
       </c>
@@ -2986,10 +2968,8 @@
       <c r="G20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>69</v>
       </c>
@@ -3011,10 +2991,8 @@
       <c r="G21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>72</v>
       </c>
@@ -3036,10 +3014,8 @@
       <c r="G22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>75</v>
       </c>
@@ -3061,10 +3037,8 @@
       <c r="G23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>76</v>
       </c>
@@ -3086,10 +3060,8 @@
       <c r="G24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>77</v>
       </c>
@@ -3111,10 +3083,8 @@
       <c r="G25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>78</v>
       </c>
@@ -3136,10 +3106,8 @@
       <c r="G26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>79</v>
       </c>
@@ -3161,10 +3129,8 @@
       <c r="G27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>80</v>
       </c>
@@ -3186,10 +3152,8 @@
       <c r="G28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="1:9" ht="61" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>81</v>
       </c>
@@ -3214,9 +3178,8 @@
       <c r="H29" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>82</v>
       </c>
@@ -3238,10 +3201,8 @@
       <c r="G30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>83</v>
       </c>
@@ -3263,10 +3224,8 @@
       <c r="G31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-    </row>
-    <row r="32" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>84</v>
       </c>
@@ -3288,10 +3247,8 @@
       <c r="G32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-    </row>
-    <row r="33" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>85</v>
       </c>
@@ -3313,10 +3270,8 @@
       <c r="G33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-    </row>
-    <row r="34" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>86</v>
       </c>
@@ -3338,10 +3293,8 @@
       <c r="G34" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>87</v>
       </c>
@@ -3363,10 +3316,8 @@
       <c r="G35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-    </row>
-    <row r="36" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>88</v>
       </c>
@@ -3388,10 +3339,8 @@
       <c r="G36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>89</v>
       </c>
@@ -3413,10 +3362,8 @@
       <c r="G37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-    </row>
-    <row r="38" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>90</v>
       </c>
@@ -3438,10 +3385,8 @@
       <c r="G38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-    </row>
-    <row r="39" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>91</v>
       </c>
@@ -3463,10 +3408,8 @@
       <c r="G39" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-    </row>
-    <row r="40" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>92</v>
       </c>
@@ -3491,9 +3434,8 @@
       <c r="H40" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="I40" s="2"/>
-    </row>
-    <row r="41" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>93</v>
       </c>
@@ -3515,10 +3457,8 @@
       <c r="G41" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-    </row>
-    <row r="42" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>94</v>
       </c>
@@ -3540,10 +3480,8 @@
       <c r="G42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-    </row>
-    <row r="43" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>95</v>
       </c>
@@ -3565,10 +3503,8 @@
       <c r="G43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-    </row>
-    <row r="44" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>96</v>
       </c>
@@ -3590,10 +3526,8 @@
       <c r="G44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-    </row>
-    <row r="45" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>97</v>
       </c>
@@ -3615,10 +3549,8 @@
       <c r="G45" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-    </row>
-    <row r="46" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>98</v>
       </c>
@@ -3640,10 +3572,8 @@
       <c r="G46" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-    </row>
-    <row r="47" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>142</v>
       </c>
@@ -3665,10 +3595,8 @@
       <c r="G47" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-    </row>
-    <row r="48" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>143</v>
       </c>
@@ -3690,10 +3618,8 @@
       <c r="G48" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-    </row>
-    <row r="49" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>144</v>
       </c>
@@ -3715,10 +3641,8 @@
       <c r="G49" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-    </row>
-    <row r="50" spans="1:9" ht="46" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>145</v>
       </c>
@@ -3740,10 +3664,8 @@
       <c r="G50" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-    </row>
-    <row r="51" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>146</v>
       </c>
@@ -3765,10 +3687,8 @@
       <c r="G51" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-    </row>
-    <row r="52" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>147</v>
       </c>
@@ -3790,10 +3710,8 @@
       <c r="G52" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-    </row>
-    <row r="53" spans="1:9" ht="61" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>148</v>
       </c>
@@ -3818,9 +3736,8 @@
       <c r="H53" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="I53" s="2"/>
-    </row>
-    <row r="54" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>149</v>
       </c>
@@ -3842,10 +3759,8 @@
       <c r="G54" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-    </row>
-    <row r="55" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>150</v>
       </c>
@@ -3867,10 +3782,8 @@
       <c r="G55" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-    </row>
-    <row r="56" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>151</v>
       </c>
@@ -3892,10 +3805,8 @@
       <c r="G56" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-    </row>
-    <row r="57" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>152</v>
       </c>
@@ -3917,10 +3828,8 @@
       <c r="G57" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-    </row>
-    <row r="58" spans="1:9" ht="61" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>153</v>
       </c>
@@ -3945,9 +3854,8 @@
       <c r="H58" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="I58" s="2"/>
-    </row>
-    <row r="59" spans="1:9" ht="46" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>154</v>
       </c>
@@ -3972,9 +3880,8 @@
       <c r="H59" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="I59" s="2"/>
-    </row>
-    <row r="60" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>154</v>
       </c>
@@ -3996,10 +3903,8 @@
       <c r="G60" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-    </row>
-    <row r="61" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>184</v>
       </c>
@@ -4021,10 +3926,8 @@
       <c r="G61" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-    </row>
-    <row r="62" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>185</v>
       </c>
@@ -4046,10 +3949,8 @@
       <c r="G62" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-    </row>
-    <row r="63" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>186</v>
       </c>
@@ -4071,10 +3972,8 @@
       <c r="G63" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-    </row>
-    <row r="64" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>187</v>
       </c>
@@ -4096,10 +3995,8 @@
       <c r="G64" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-    </row>
-    <row r="65" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>188</v>
       </c>
@@ -4121,10 +4018,8 @@
       <c r="G65" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-    </row>
-    <row r="66" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>189</v>
       </c>
@@ -4146,10 +4041,8 @@
       <c r="G66" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
-    </row>
-    <row r="67" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>190</v>
       </c>
@@ -4171,10 +4064,8 @@
       <c r="G67" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-    </row>
-    <row r="68" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>191</v>
       </c>
@@ -4196,10 +4087,8 @@
       <c r="G68" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
-    </row>
-    <row r="69" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>192</v>
       </c>
@@ -4221,10 +4110,8 @@
       <c r="G69" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
-    </row>
-    <row r="70" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>213</v>
       </c>
@@ -4246,10 +4133,8 @@
       <c r="G70" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
-    </row>
-    <row r="71" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>214</v>
       </c>
@@ -4271,10 +4156,8 @@
       <c r="G71" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H71" s="2"/>
-      <c r="I71" s="2"/>
-    </row>
-    <row r="72" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>215</v>
       </c>
@@ -4296,10 +4179,8 @@
       <c r="G72" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H72" s="2"/>
-      <c r="I72" s="2"/>
-    </row>
-    <row r="73" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>216</v>
       </c>
@@ -4321,10 +4202,8 @@
       <c r="G73" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-    </row>
-    <row r="74" spans="1:9" ht="46" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>217</v>
       </c>
@@ -4346,10 +4225,8 @@
       <c r="G74" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H74" s="2"/>
-      <c r="I74" s="2"/>
-    </row>
-    <row r="75" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>218</v>
       </c>
@@ -4371,10 +4248,8 @@
       <c r="G75" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H75" s="2"/>
-      <c r="I75" s="2"/>
-    </row>
-    <row r="76" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>231</v>
       </c>
@@ -4396,10 +4271,8 @@
       <c r="G76" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H76" s="2"/>
-      <c r="I76" s="2"/>
-    </row>
-    <row r="77" spans="1:9" ht="46" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>232</v>
       </c>
@@ -4424,9 +4297,8 @@
       <c r="H77" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="I77" s="2"/>
-    </row>
-    <row r="78" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>233</v>
       </c>
@@ -4448,10 +4320,8 @@
       <c r="G78" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H78" s="2"/>
-      <c r="I78" s="2"/>
-    </row>
-    <row r="79" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>234</v>
       </c>
@@ -4473,10 +4343,8 @@
       <c r="G79" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H79" s="2"/>
-      <c r="I79" s="2"/>
-    </row>
-    <row r="80" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>235</v>
       </c>
@@ -4498,10 +4366,8 @@
       <c r="G80" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H80" s="2"/>
-      <c r="I80" s="2"/>
-    </row>
-    <row r="81" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>236</v>
       </c>
@@ -4523,10 +4389,8 @@
       <c r="G81" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H81" s="2"/>
-      <c r="I81" s="2"/>
-    </row>
-    <row r="82" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>254</v>
       </c>
@@ -4548,10 +4412,8 @@
       <c r="G82" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H82" s="2"/>
-      <c r="I82" s="2"/>
-    </row>
-    <row r="83" spans="1:9" ht="121" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:9" ht="170" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>255</v>
       </c>
@@ -4573,12 +4435,11 @@
       <c r="G83" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="H83" s="2"/>
       <c r="I83" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>261</v>
       </c>
@@ -4600,10 +4461,8 @@
       <c r="G84" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="H84" s="2"/>
-      <c r="I84" s="2"/>
-    </row>
-    <row r="85" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>263</v>
       </c>
@@ -4625,10 +4484,8 @@
       <c r="G85" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
-    </row>
-    <row r="86" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>264</v>
       </c>
@@ -4650,12 +4507,11 @@
       <c r="G86" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="H86" s="2"/>
       <c r="I86" s="2" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>264</v>
       </c>
@@ -4677,12 +4533,11 @@
       <c r="G87" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="H87" s="2"/>
       <c r="I87" s="2" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="46" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>217</v>
       </c>
@@ -4704,12 +4559,11 @@
       <c r="G88" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="H88" s="2"/>
       <c r="I88" s="2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>265</v>
       </c>
@@ -4731,10 +4585,8 @@
       <c r="G89" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
-    </row>
-    <row r="90" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>266</v>
       </c>
@@ -4756,10 +4608,8 @@
       <c r="G90" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="H90" s="2"/>
-      <c r="I90" s="2"/>
-    </row>
-    <row r="91" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>267</v>
       </c>
@@ -4781,10 +4631,8 @@
       <c r="G91" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="H91" s="2"/>
-      <c r="I91" s="2"/>
-    </row>
-    <row r="92" spans="1:9" ht="46" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>268</v>
       </c>
@@ -4806,10 +4654,8 @@
       <c r="G92" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="H92" s="2"/>
-      <c r="I92" s="2"/>
-    </row>
-    <row r="93" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>269</v>
       </c>
@@ -4831,10 +4677,8 @@
       <c r="G93" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="H93" s="2"/>
-      <c r="I93" s="2"/>
-    </row>
-    <row r="94" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>270</v>
       </c>
@@ -4856,10 +4700,8 @@
       <c r="G94" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="H94" s="2"/>
-      <c r="I94" s="2"/>
-    </row>
-    <row r="95" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>271</v>
       </c>
@@ -4881,10 +4723,8 @@
       <c r="G95" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="H95" s="2"/>
-      <c r="I95" s="2"/>
-    </row>
-    <row r="96" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>272</v>
       </c>
@@ -4906,10 +4746,8 @@
       <c r="G96" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="H96" s="2"/>
-      <c r="I96" s="2"/>
-    </row>
-    <row r="97" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>273</v>
       </c>
@@ -4931,10 +4769,8 @@
       <c r="G97" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="H97" s="2"/>
-      <c r="I97" s="2"/>
-    </row>
-    <row r="98" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>274</v>
       </c>
@@ -4956,10 +4792,8 @@
       <c r="G98" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="H98" s="2"/>
-      <c r="I98" s="2"/>
-    </row>
-    <row r="99" spans="1:9" ht="76" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>275</v>
       </c>
@@ -4981,12 +4815,11 @@
       <c r="G99" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="H99" s="2"/>
       <c r="I99" s="2" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>276</v>
       </c>
@@ -5008,10 +4841,8 @@
       <c r="G100" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="H100" s="2"/>
-      <c r="I100" s="2"/>
-    </row>
-    <row r="101" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>277</v>
       </c>
@@ -5033,10 +4864,8 @@
       <c r="G101" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="H101" s="2"/>
-      <c r="I101" s="2"/>
-    </row>
-    <row r="102" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="102" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>311</v>
       </c>
@@ -5058,10 +4887,8 @@
       <c r="G102" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="H102" s="2"/>
-      <c r="I102" s="2"/>
-    </row>
-    <row r="103" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="103" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>312</v>
       </c>
@@ -5083,10 +4910,8 @@
       <c r="G103" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="H103" s="2"/>
-      <c r="I103" s="2"/>
-    </row>
-    <row r="104" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="104" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>313</v>
       </c>
@@ -5108,10 +4933,8 @@
       <c r="G104" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="H104" s="2"/>
-      <c r="I104" s="2"/>
-    </row>
-    <row r="105" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>314</v>
       </c>
@@ -5133,10 +4956,8 @@
       <c r="G105" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="H105" s="2"/>
-      <c r="I105" s="2"/>
-    </row>
-    <row r="106" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="106" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>315</v>
       </c>
@@ -5158,10 +4979,8 @@
       <c r="G106" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="H106" s="2"/>
-      <c r="I106" s="2"/>
-    </row>
-    <row r="107" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>316</v>
       </c>
@@ -5183,10 +5002,8 @@
       <c r="G107" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="H107" s="2"/>
-      <c r="I107" s="2"/>
-    </row>
-    <row r="108" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>317</v>
       </c>
@@ -5208,10 +5025,8 @@
       <c r="G108" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="H108" s="2"/>
-      <c r="I108" s="2"/>
-    </row>
-    <row r="109" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="109" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>318</v>
       </c>
@@ -5233,10 +5048,8 @@
       <c r="G109" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="H109" s="2"/>
-      <c r="I109" s="2"/>
-    </row>
-    <row r="110" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="110" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>319</v>
       </c>
@@ -5258,10 +5071,8 @@
       <c r="G110" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="H110" s="2"/>
-      <c r="I110" s="2"/>
-    </row>
-    <row r="111" spans="1:9" ht="61" x14ac:dyDescent="0.2">
+    </row>
+    <row r="111" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>320</v>
       </c>
@@ -5283,10 +5094,8 @@
       <c r="G111" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="H111" s="2"/>
-      <c r="I111" s="2"/>
-    </row>
-    <row r="112" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="112" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>321</v>
       </c>
@@ -5308,10 +5117,8 @@
       <c r="G112" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="H112" s="2"/>
-      <c r="I112" s="2"/>
-    </row>
-    <row r="113" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>680</v>
       </c>
@@ -5333,10 +5140,8 @@
       <c r="G113" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="H113" s="2"/>
-      <c r="I113" s="2"/>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="114" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>385</v>
       </c>
@@ -5355,11 +5160,8 @@
       <c r="F114" s="2">
         <v>1</v>
       </c>
-      <c r="G114" s="2"/>
-      <c r="H114" s="2"/>
-      <c r="I114" s="2"/>
-    </row>
-    <row r="115" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="115" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>386</v>
       </c>
@@ -5378,11 +5180,8 @@
       <c r="F115" s="2">
         <v>2</v>
       </c>
-      <c r="G115" s="2"/>
-      <c r="H115" s="2"/>
-      <c r="I115" s="2"/>
-    </row>
-    <row r="116" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="116" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>391</v>
       </c>
@@ -5401,11 +5200,8 @@
       <c r="F116" s="2">
         <v>2</v>
       </c>
-      <c r="G116" s="2"/>
-      <c r="H116" s="2"/>
-      <c r="I116" s="2"/>
-    </row>
-    <row r="117" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="117" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
         <v>190</v>
       </c>
@@ -5424,11 +5220,8 @@
       <c r="F117" s="2">
         <v>2</v>
       </c>
-      <c r="G117" s="2"/>
-      <c r="H117" s="2"/>
-      <c r="I117" s="2"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="118" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>395</v>
       </c>
@@ -5447,11 +5240,8 @@
       <c r="F118" s="2">
         <v>1</v>
       </c>
-      <c r="G118" s="2"/>
-      <c r="H118" s="2"/>
-      <c r="I118" s="2"/>
-    </row>
-    <row r="119" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="119" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>398</v>
       </c>
@@ -5470,11 +5260,8 @@
       <c r="F119" s="2">
         <v>2</v>
       </c>
-      <c r="G119" s="2"/>
-      <c r="H119" s="2"/>
-      <c r="I119" s="2"/>
-    </row>
-    <row r="120" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="120" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>401</v>
       </c>
@@ -5493,11 +5280,8 @@
       <c r="F120" s="2">
         <v>3</v>
       </c>
-      <c r="G120" s="2"/>
-      <c r="H120" s="2"/>
-      <c r="I120" s="2"/>
-    </row>
-    <row r="121" spans="1:9" ht="61" x14ac:dyDescent="0.2">
+    </row>
+    <row r="121" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>404</v>
       </c>
@@ -5516,13 +5300,11 @@
       <c r="F121" s="2">
         <v>2</v>
       </c>
-      <c r="G121" s="2"/>
       <c r="H121" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="I121" s="2"/>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="122" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>408</v>
       </c>
@@ -5541,11 +5323,8 @@
       <c r="F122" s="2">
         <v>1</v>
       </c>
-      <c r="G122" s="2"/>
-      <c r="H122" s="2"/>
-      <c r="I122" s="2"/>
-    </row>
-    <row r="123" spans="1:9" ht="46" x14ac:dyDescent="0.2">
+    </row>
+    <row r="123" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>75</v>
       </c>
@@ -5564,11 +5343,8 @@
       <c r="F123" s="2">
         <v>3</v>
       </c>
-      <c r="G123" s="2"/>
-      <c r="H123" s="2"/>
-      <c r="I123" s="2"/>
-    </row>
-    <row r="124" spans="1:9" ht="76" x14ac:dyDescent="0.2">
+    </row>
+    <row r="124" spans="1:8" ht="119" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>411</v>
       </c>
@@ -5587,13 +5363,11 @@
       <c r="F124" s="2">
         <v>4</v>
       </c>
-      <c r="G124" s="2"/>
       <c r="H124" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="I124" s="2"/>
-    </row>
-    <row r="125" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="125" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>412</v>
       </c>
@@ -5612,11 +5386,8 @@
       <c r="F125" s="2">
         <v>2</v>
       </c>
-      <c r="G125" s="2"/>
-      <c r="H125" s="2"/>
-      <c r="I125" s="2"/>
-    </row>
-    <row r="126" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="126" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>413</v>
       </c>
@@ -5635,11 +5406,8 @@
       <c r="F126" s="2">
         <v>2</v>
       </c>
-      <c r="G126" s="2"/>
-      <c r="H126" s="2"/>
-      <c r="I126" s="2"/>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="127" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>423</v>
       </c>
@@ -5658,11 +5426,8 @@
       <c r="F127" s="2">
         <v>1</v>
       </c>
-      <c r="G127" s="2"/>
-      <c r="H127" s="2"/>
-      <c r="I127" s="2"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="128" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>425</v>
       </c>
@@ -5681,11 +5446,8 @@
       <c r="F128" s="2">
         <v>1</v>
       </c>
-      <c r="G128" s="2"/>
-      <c r="H128" s="2"/>
-      <c r="I128" s="2"/>
-    </row>
-    <row r="129" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="129" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
         <v>231</v>
       </c>
@@ -5704,11 +5466,8 @@
       <c r="F129" s="2">
         <v>2</v>
       </c>
-      <c r="G129" s="2"/>
-      <c r="H129" s="2"/>
-      <c r="I129" s="2"/>
-    </row>
-    <row r="130" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="130" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
         <v>88</v>
       </c>
@@ -5727,11 +5486,8 @@
       <c r="F130" s="2">
         <v>2</v>
       </c>
-      <c r="G130" s="2"/>
-      <c r="H130" s="2"/>
-      <c r="I130" s="2"/>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="131" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>432</v>
       </c>
@@ -5750,11 +5506,8 @@
       <c r="F131" s="2">
         <v>1</v>
       </c>
-      <c r="G131" s="2"/>
-      <c r="H131" s="2"/>
-      <c r="I131" s="2"/>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="132" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>435</v>
       </c>
@@ -5773,11 +5526,8 @@
       <c r="F132" s="2">
         <v>1</v>
       </c>
-      <c r="G132" s="2"/>
-      <c r="H132" s="2"/>
-      <c r="I132" s="2"/>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="133" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>82</v>
       </c>
@@ -5796,11 +5546,8 @@
       <c r="F133" s="2">
         <v>1</v>
       </c>
-      <c r="G133" s="2"/>
-      <c r="H133" s="2"/>
-      <c r="I133" s="2"/>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="134" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>436</v>
       </c>
@@ -5819,11 +5566,8 @@
       <c r="F134" s="2">
         <v>1</v>
       </c>
-      <c r="G134" s="2"/>
-      <c r="H134" s="2"/>
-      <c r="I134" s="2"/>
-    </row>
-    <row r="135" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="135" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
         <v>93</v>
       </c>
@@ -5842,11 +5586,8 @@
       <c r="F135" s="2">
         <v>2</v>
       </c>
-      <c r="G135" s="2"/>
-      <c r="H135" s="2"/>
-      <c r="I135" s="2"/>
-    </row>
-    <row r="136" spans="1:9" ht="46" x14ac:dyDescent="0.2">
+    </row>
+    <row r="136" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>435</v>
       </c>
@@ -5865,13 +5606,11 @@
       <c r="F136" s="2">
         <v>2</v>
       </c>
-      <c r="G136" s="2"/>
       <c r="H136" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="I136" s="2"/>
-    </row>
-    <row r="137" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="137" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>436</v>
       </c>
@@ -5890,11 +5629,8 @@
       <c r="F137" s="2">
         <v>2</v>
       </c>
-      <c r="G137" s="2"/>
-      <c r="H137" s="2"/>
-      <c r="I137" s="2"/>
-    </row>
-    <row r="138" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="138" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>93</v>
       </c>
@@ -5913,11 +5649,8 @@
       <c r="F138" s="2">
         <v>2</v>
       </c>
-      <c r="G138" s="2"/>
-      <c r="H138" s="2"/>
-      <c r="I138" s="2"/>
-    </row>
-    <row r="139" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="139" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>444</v>
       </c>
@@ -5936,13 +5669,11 @@
       <c r="F139" s="2">
         <v>2</v>
       </c>
-      <c r="G139" s="2"/>
       <c r="H139" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="I139" s="2"/>
-    </row>
-    <row r="140" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="140" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>444</v>
       </c>
@@ -5961,11 +5692,8 @@
       <c r="F140" s="2">
         <v>2</v>
       </c>
-      <c r="G140" s="2"/>
-      <c r="H140" s="2"/>
-      <c r="I140" s="2"/>
-    </row>
-    <row r="141" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="141" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>444</v>
       </c>
@@ -5984,11 +5712,8 @@
       <c r="F141" s="2">
         <v>2</v>
       </c>
-      <c r="G141" s="2"/>
-      <c r="H141" s="2"/>
-      <c r="I141" s="2"/>
-    </row>
-    <row r="142" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="142" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>455</v>
       </c>
@@ -6007,11 +5732,8 @@
       <c r="F142" s="2">
         <v>2</v>
       </c>
-      <c r="G142" s="2"/>
-      <c r="H142" s="2"/>
-      <c r="I142" s="2"/>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="143" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>269</v>
       </c>
@@ -6030,11 +5752,8 @@
       <c r="F143" s="2">
         <v>1</v>
       </c>
-      <c r="G143" s="2"/>
-      <c r="H143" s="2"/>
-      <c r="I143" s="2"/>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="144" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>461</v>
       </c>
@@ -6053,11 +5772,8 @@
       <c r="F144" s="2">
         <v>1</v>
       </c>
-      <c r="G144" s="2"/>
-      <c r="H144" s="2"/>
-      <c r="I144" s="2"/>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="145" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>464</v>
       </c>
@@ -6076,11 +5792,8 @@
       <c r="F145" s="2">
         <v>1</v>
       </c>
-      <c r="G145" s="2"/>
-      <c r="H145" s="2"/>
-      <c r="I145" s="2"/>
-    </row>
-    <row r="146" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="146" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>467</v>
       </c>
@@ -6099,11 +5812,8 @@
       <c r="F146" s="2">
         <v>2</v>
       </c>
-      <c r="G146" s="2"/>
-      <c r="H146" s="2"/>
-      <c r="I146" s="2"/>
-    </row>
-    <row r="147" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="147" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>470</v>
       </c>
@@ -6122,11 +5832,8 @@
       <c r="F147" s="2">
         <v>2</v>
       </c>
-      <c r="G147" s="2"/>
-      <c r="H147" s="2"/>
-      <c r="I147" s="2"/>
-    </row>
-    <row r="148" spans="1:9" ht="91" x14ac:dyDescent="0.2">
+    </row>
+    <row r="148" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
         <v>461</v>
       </c>
@@ -6145,13 +5852,11 @@
       <c r="F148" s="2">
         <v>2</v>
       </c>
-      <c r="G148" s="2"/>
       <c r="H148" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="I148" s="2"/>
-    </row>
-    <row r="149" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="149" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
         <v>461</v>
       </c>
@@ -6170,11 +5875,8 @@
       <c r="F149" s="2">
         <v>2</v>
       </c>
-      <c r="G149" s="2"/>
-      <c r="H149" s="2"/>
-      <c r="I149" s="2"/>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="150" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>471</v>
       </c>
@@ -6193,11 +5895,8 @@
       <c r="F150" s="2">
         <v>1</v>
       </c>
-      <c r="G150" s="2"/>
-      <c r="H150" s="2"/>
-      <c r="I150" s="2"/>
-    </row>
-    <row r="151" spans="1:9" ht="46" x14ac:dyDescent="0.2">
+    </row>
+    <row r="151" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>479</v>
       </c>
@@ -6216,13 +5915,11 @@
       <c r="F151" s="2">
         <v>4</v>
       </c>
-      <c r="G151" s="2"/>
       <c r="H151" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="I151" s="2"/>
-    </row>
-    <row r="152" spans="1:9" ht="46" x14ac:dyDescent="0.2">
+    </row>
+    <row r="152" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>484</v>
       </c>
@@ -6241,11 +5938,8 @@
       <c r="F152" s="2">
         <v>2</v>
       </c>
-      <c r="G152" s="2"/>
-      <c r="H152" s="2"/>
-      <c r="I152" s="2"/>
-    </row>
-    <row r="153" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="153" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>487</v>
       </c>
@@ -6264,11 +5958,8 @@
       <c r="F153" s="2">
         <v>3</v>
       </c>
-      <c r="G153" s="2"/>
-      <c r="H153" s="2"/>
-      <c r="I153" s="2"/>
-    </row>
-    <row r="154" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="154" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>489</v>
       </c>
@@ -6287,13 +5978,11 @@
       <c r="F154" s="2">
         <v>2</v>
       </c>
-      <c r="G154" s="2"/>
       <c r="H154" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="I154" s="2"/>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="155" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>494</v>
       </c>
@@ -6312,11 +6001,8 @@
       <c r="F155" s="2">
         <v>1</v>
       </c>
-      <c r="G155" s="2"/>
-      <c r="H155" s="2"/>
-      <c r="I155" s="2"/>
-    </row>
-    <row r="156" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="156" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
         <v>154</v>
       </c>
@@ -6335,11 +6021,8 @@
       <c r="F156" s="2">
         <v>2</v>
       </c>
-      <c r="G156" s="2"/>
-      <c r="H156" s="2"/>
-      <c r="I156" s="2"/>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="157" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>499</v>
       </c>
@@ -6358,11 +6041,8 @@
       <c r="F157" s="2">
         <v>1</v>
       </c>
-      <c r="G157" s="2"/>
-      <c r="H157" s="2"/>
-      <c r="I157" s="2"/>
-    </row>
-    <row r="158" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="158" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>502</v>
       </c>
@@ -6381,13 +6061,11 @@
       <c r="F158" s="2">
         <v>1</v>
       </c>
-      <c r="G158" s="2"/>
       <c r="H158" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="I158" s="2"/>
-    </row>
-    <row r="159" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="159" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>505</v>
       </c>
@@ -6406,11 +6084,8 @@
       <c r="F159" s="2">
         <v>2</v>
       </c>
-      <c r="G159" s="2"/>
-      <c r="H159" s="2"/>
-      <c r="I159" s="2"/>
-    </row>
-    <row r="160" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="160" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>507</v>
       </c>
@@ -6429,11 +6104,8 @@
       <c r="F160" s="2">
         <v>2</v>
       </c>
-      <c r="G160" s="2"/>
-      <c r="H160" s="2"/>
-      <c r="I160" s="2"/>
-    </row>
-    <row r="161" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="161" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>510</v>
       </c>
@@ -6452,11 +6124,8 @@
       <c r="F161" s="2">
         <v>2</v>
       </c>
-      <c r="G161" s="2"/>
-      <c r="H161" s="2"/>
-      <c r="I161" s="2"/>
-    </row>
-    <row r="162" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="162" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
         <v>236</v>
       </c>
@@ -6475,11 +6144,8 @@
       <c r="F162" s="2">
         <v>2</v>
       </c>
-      <c r="G162" s="2"/>
-      <c r="H162" s="2"/>
-      <c r="I162" s="2"/>
-    </row>
-    <row r="163" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="163" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>512</v>
       </c>
@@ -6498,11 +6164,8 @@
       <c r="F163" s="2">
         <v>2</v>
       </c>
-      <c r="G163" s="2"/>
-      <c r="H163" s="2"/>
-      <c r="I163" s="2"/>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="164" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>517</v>
       </c>
@@ -6521,11 +6184,8 @@
       <c r="F164" s="2">
         <v>1</v>
       </c>
-      <c r="G164" s="2"/>
-      <c r="H164" s="2"/>
-      <c r="I164" s="2"/>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="165" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>520</v>
       </c>
@@ -6544,11 +6204,8 @@
       <c r="F165" s="2">
         <v>1</v>
       </c>
-      <c r="G165" s="2"/>
-      <c r="H165" s="2"/>
-      <c r="I165" s="2"/>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="166" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>523</v>
       </c>
@@ -6567,11 +6224,8 @@
       <c r="F166" s="2">
         <v>1</v>
       </c>
-      <c r="G166" s="2"/>
-      <c r="H166" s="2"/>
-      <c r="I166" s="2"/>
-    </row>
-    <row r="167" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="167" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>526</v>
       </c>
@@ -6590,11 +6244,8 @@
       <c r="F167" s="2">
         <v>2</v>
       </c>
-      <c r="G167" s="2"/>
-      <c r="H167" s="2"/>
-      <c r="I167" s="2"/>
-    </row>
-    <row r="168" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="168" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
         <v>86</v>
       </c>
@@ -6613,11 +6264,8 @@
       <c r="F168" s="2">
         <v>2</v>
       </c>
-      <c r="G168" s="2"/>
-      <c r="H168" s="2"/>
-      <c r="I168" s="2"/>
-    </row>
-    <row r="169" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="169" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A169" s="4" t="s">
         <v>86</v>
       </c>
@@ -6636,11 +6284,8 @@
       <c r="F169" s="2">
         <v>2</v>
       </c>
-      <c r="G169" s="2"/>
-      <c r="H169" s="2"/>
-      <c r="I169" s="2"/>
-    </row>
-    <row r="170" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="170" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>531</v>
       </c>
@@ -6659,11 +6304,8 @@
       <c r="F170" s="2">
         <v>2</v>
       </c>
-      <c r="G170" s="2"/>
-      <c r="H170" s="2"/>
-      <c r="I170" s="2"/>
-    </row>
-    <row r="171" spans="1:9" ht="121" x14ac:dyDescent="0.2">
+    </row>
+    <row r="171" spans="1:8" ht="136" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>534</v>
       </c>
@@ -6682,13 +6324,11 @@
       <c r="F171" s="2">
         <v>1</v>
       </c>
-      <c r="G171" s="2"/>
       <c r="H171" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="I171" s="2"/>
-    </row>
-    <row r="172" spans="1:9" ht="46" x14ac:dyDescent="0.2">
+    </row>
+    <row r="172" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A172" s="4" t="s">
         <v>45</v>
       </c>
@@ -6707,11 +6347,8 @@
       <c r="F172" s="2">
         <v>3</v>
       </c>
-      <c r="G172" s="2"/>
-      <c r="H172" s="2"/>
-      <c r="I172" s="2"/>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="173" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>540</v>
       </c>
@@ -6730,11 +6367,8 @@
       <c r="F173" s="2">
         <v>1</v>
       </c>
-      <c r="G173" s="2"/>
-      <c r="H173" s="2"/>
-      <c r="I173" s="2"/>
-    </row>
-    <row r="174" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="174" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>543</v>
       </c>
@@ -6753,11 +6387,8 @@
       <c r="F174" s="2">
         <v>1</v>
       </c>
-      <c r="G174" s="2"/>
-      <c r="H174" s="2"/>
-      <c r="I174" s="2"/>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="175" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>546</v>
       </c>
@@ -6776,11 +6407,8 @@
       <c r="F175" s="2">
         <v>1</v>
       </c>
-      <c r="G175" s="2"/>
-      <c r="H175" s="2"/>
-      <c r="I175" s="2"/>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="176" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
         <v>549</v>
       </c>
@@ -6799,11 +6427,8 @@
       <c r="F176" s="2">
         <v>2</v>
       </c>
-      <c r="G176" s="2"/>
-      <c r="H176" s="2"/>
-      <c r="I176" s="2"/>
-    </row>
-    <row r="177" spans="1:9" ht="46" x14ac:dyDescent="0.2">
+    </row>
+    <row r="177" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A177" s="4" t="s">
         <v>315</v>
       </c>
@@ -6822,13 +6447,11 @@
       <c r="F177" s="2">
         <v>2</v>
       </c>
-      <c r="G177" s="2"/>
       <c r="H177" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="I177" s="2"/>
-    </row>
-    <row r="178" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="178" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
         <v>555</v>
       </c>
@@ -6847,11 +6470,8 @@
       <c r="F178" s="2">
         <v>2</v>
       </c>
-      <c r="G178" s="2"/>
-      <c r="H178" s="2"/>
-      <c r="I178" s="2"/>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="179" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
         <v>558</v>
       </c>
@@ -6870,11 +6490,8 @@
       <c r="F179" s="2">
         <v>1</v>
       </c>
-      <c r="G179" s="2"/>
-      <c r="H179" s="2"/>
-      <c r="I179" s="2"/>
-    </row>
-    <row r="180" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="180" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
         <v>561</v>
       </c>
@@ -6893,11 +6510,8 @@
       <c r="F180" s="2">
         <v>2</v>
       </c>
-      <c r="G180" s="2"/>
-      <c r="H180" s="2"/>
-      <c r="I180" s="2"/>
-    </row>
-    <row r="181" spans="1:9" ht="46" x14ac:dyDescent="0.2">
+    </row>
+    <row r="181" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A181" s="4" t="s">
         <v>145</v>
       </c>
@@ -6916,11 +6530,8 @@
       <c r="F181" s="2">
         <v>3</v>
       </c>
-      <c r="G181" s="2"/>
-      <c r="H181" s="2"/>
-      <c r="I181" s="2"/>
-    </row>
-    <row r="182" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="182" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
         <v>564</v>
       </c>
@@ -6939,11 +6550,8 @@
       <c r="F182" s="2">
         <v>2</v>
       </c>
-      <c r="G182" s="2"/>
-      <c r="H182" s="2"/>
-      <c r="I182" s="2"/>
-    </row>
-    <row r="183" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="183" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A183" s="4" t="s">
         <v>231</v>
       </c>
@@ -6962,11 +6570,8 @@
       <c r="F183" s="2">
         <v>2</v>
       </c>
-      <c r="G183" s="2"/>
-      <c r="H183" s="2"/>
-      <c r="I183" s="2"/>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="184" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
         <v>571</v>
       </c>
@@ -6985,11 +6590,8 @@
       <c r="F184" s="2">
         <v>1</v>
       </c>
-      <c r="G184" s="2"/>
-      <c r="H184" s="2"/>
-      <c r="I184" s="2"/>
-    </row>
-    <row r="185" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="185" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A185" s="4" t="s">
         <v>263</v>
       </c>
@@ -7008,11 +6610,8 @@
       <c r="F185" s="2">
         <v>2</v>
       </c>
-      <c r="G185" s="2"/>
-      <c r="H185" s="2"/>
-      <c r="I185" s="2"/>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="186" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
         <v>576</v>
       </c>
@@ -7031,11 +6630,8 @@
       <c r="F186" s="2">
         <v>1</v>
       </c>
-      <c r="G186" s="2"/>
-      <c r="H186" s="2"/>
-      <c r="I186" s="2"/>
-    </row>
-    <row r="187" spans="1:9" ht="46" x14ac:dyDescent="0.2">
+    </row>
+    <row r="187" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
         <v>578</v>
       </c>
@@ -7054,11 +6650,8 @@
       <c r="F187" s="2">
         <v>3</v>
       </c>
-      <c r="G187" s="2"/>
-      <c r="H187" s="2"/>
-      <c r="I187" s="2"/>
-    </row>
-    <row r="188" spans="1:9" ht="61" x14ac:dyDescent="0.2">
+    </row>
+    <row r="188" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
         <v>583</v>
       </c>
@@ -7077,13 +6670,11 @@
       <c r="F188" s="2">
         <v>4</v>
       </c>
-      <c r="G188" s="2"/>
       <c r="H188" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="I188" s="2"/>
-    </row>
-    <row r="189" spans="1:9" ht="61" x14ac:dyDescent="0.2">
+    </row>
+    <row r="189" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
         <v>584</v>
       </c>
@@ -7102,13 +6693,11 @@
       <c r="F189" s="2">
         <v>4</v>
       </c>
-      <c r="G189" s="2"/>
       <c r="H189" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="I189" s="2"/>
-    </row>
-    <row r="190" spans="1:9" ht="46" x14ac:dyDescent="0.2">
+    </row>
+    <row r="190" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A190" s="4" t="s">
         <v>218</v>
       </c>
@@ -7127,13 +6716,11 @@
       <c r="F190" s="2">
         <v>2</v>
       </c>
-      <c r="G190" s="2"/>
       <c r="H190" s="2" t="s">
         <v>616</v>
       </c>
-      <c r="I190" s="2"/>
-    </row>
-    <row r="191" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="191" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A191" s="4" t="s">
         <v>261</v>
       </c>
@@ -7152,11 +6739,8 @@
       <c r="F191" s="2">
         <v>2</v>
       </c>
-      <c r="G191" s="2"/>
-      <c r="H191" s="2"/>
-      <c r="I191" s="2"/>
-    </row>
-    <row r="192" spans="1:9" ht="61" x14ac:dyDescent="0.2">
+    </row>
+    <row r="192" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
         <v>588</v>
       </c>
@@ -7175,11 +6759,8 @@
       <c r="F192" s="2">
         <v>4</v>
       </c>
-      <c r="G192" s="2"/>
-      <c r="H192" s="2"/>
-      <c r="I192" s="2"/>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="193" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
         <v>593</v>
       </c>
@@ -7198,11 +6779,8 @@
       <c r="F193" s="2">
         <v>1</v>
       </c>
-      <c r="G193" s="2"/>
-      <c r="H193" s="2"/>
-      <c r="I193" s="2"/>
-    </row>
-    <row r="194" spans="1:9" ht="46" x14ac:dyDescent="0.2">
+    </row>
+    <row r="194" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A194" s="2" t="s">
         <v>594</v>
       </c>
@@ -7221,11 +6799,8 @@
       <c r="F194" s="2">
         <v>3</v>
       </c>
-      <c r="G194" s="2"/>
-      <c r="H194" s="2"/>
-      <c r="I194" s="2"/>
-    </row>
-    <row r="195" spans="1:9" ht="46" x14ac:dyDescent="0.2">
+    </row>
+    <row r="195" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
         <v>599</v>
       </c>
@@ -7244,11 +6819,8 @@
       <c r="F195" s="2">
         <v>3</v>
       </c>
-      <c r="G195" s="2"/>
-      <c r="H195" s="2"/>
-      <c r="I195" s="2"/>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="196" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A196" s="4" t="s">
         <v>144</v>
       </c>
@@ -7267,11 +6839,8 @@
       <c r="F196" s="2">
         <v>1</v>
       </c>
-      <c r="G196" s="2"/>
-      <c r="H196" s="2"/>
-      <c r="I196" s="2"/>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="197" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
         <v>602</v>
       </c>
@@ -7290,11 +6859,8 @@
       <c r="F197" s="2">
         <v>1</v>
       </c>
-      <c r="G197" s="2"/>
-      <c r="H197" s="2"/>
-      <c r="I197" s="2"/>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="198" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
         <v>605</v>
       </c>
@@ -7313,11 +6879,8 @@
       <c r="F198" s="2">
         <v>2</v>
       </c>
-      <c r="G198" s="2"/>
-      <c r="H198" s="2"/>
-      <c r="I198" s="2"/>
-    </row>
-    <row r="199" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="199" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A199" s="4" t="s">
         <v>77</v>
       </c>
@@ -7336,11 +6899,8 @@
       <c r="F199" s="2">
         <v>2</v>
       </c>
-      <c r="G199" s="2"/>
-      <c r="H199" s="2"/>
-      <c r="I199" s="2"/>
-    </row>
-    <row r="200" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="200" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A200" s="4" t="s">
         <v>77</v>
       </c>
@@ -7359,11 +6919,8 @@
       <c r="F200" s="2">
         <v>2</v>
       </c>
-      <c r="G200" s="2"/>
-      <c r="H200" s="2"/>
-      <c r="I200" s="2"/>
-    </row>
-    <row r="201" spans="1:9" ht="76" x14ac:dyDescent="0.2">
+    </row>
+    <row r="201" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
         <v>609</v>
       </c>
@@ -7382,13 +6939,11 @@
       <c r="F201" s="2">
         <v>5</v>
       </c>
-      <c r="G201" s="2"/>
       <c r="H201" s="2" t="s">
         <v>612</v>
       </c>
-      <c r="I201" s="2"/>
-    </row>
-    <row r="202" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="202" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
         <v>615</v>
       </c>
@@ -7407,11 +6962,8 @@
       <c r="F202" s="2">
         <v>2</v>
       </c>
-      <c r="G202" s="2"/>
-      <c r="H202" s="2"/>
-      <c r="I202" s="2"/>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="203" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
         <v>623</v>
       </c>
@@ -7430,11 +6982,8 @@
       <c r="F203" s="2">
         <v>1</v>
       </c>
-      <c r="G203" s="2"/>
-      <c r="H203" s="2"/>
-      <c r="I203" s="2"/>
-    </row>
-    <row r="204" spans="1:9" ht="61" x14ac:dyDescent="0.2">
+    </row>
+    <row r="204" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
         <v>626</v>
       </c>
@@ -7453,13 +7002,11 @@
       <c r="F204" s="2">
         <v>4</v>
       </c>
-      <c r="G204" s="2"/>
       <c r="H204" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="I204" s="2"/>
-    </row>
-    <row r="205" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="205" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
         <v>630</v>
       </c>
@@ -7478,11 +7025,8 @@
       <c r="F205" s="2">
         <v>2</v>
       </c>
-      <c r="G205" s="2"/>
-      <c r="H205" s="2"/>
-      <c r="I205" s="2"/>
-    </row>
-    <row r="206" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="206" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A206" s="4" t="s">
         <v>186</v>
       </c>
@@ -7501,11 +7045,8 @@
       <c r="F206" s="2">
         <v>2</v>
       </c>
-      <c r="G206" s="2"/>
-      <c r="H206" s="2"/>
-      <c r="I206" s="2"/>
-    </row>
-    <row r="207" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="207" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A207" s="4" t="s">
         <v>186</v>
       </c>
@@ -7524,11 +7065,8 @@
       <c r="F207" s="2">
         <v>2</v>
       </c>
-      <c r="G207" s="2"/>
-      <c r="H207" s="2"/>
-      <c r="I207" s="2"/>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="208" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A208" s="4" t="s">
         <v>214</v>
       </c>
@@ -7547,11 +7085,8 @@
       <c r="F208" s="2">
         <v>2</v>
       </c>
-      <c r="G208" s="2"/>
-      <c r="H208" s="2"/>
-      <c r="I208" s="2"/>
-    </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="209" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A209" s="4" t="s">
         <v>214</v>
       </c>
@@ -7570,11 +7105,8 @@
       <c r="F209" s="2">
         <v>2</v>
       </c>
-      <c r="G209" s="2"/>
-      <c r="H209" s="2"/>
-      <c r="I209" s="2"/>
-    </row>
-    <row r="210" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="210" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A210" s="2" t="s">
         <v>638</v>
       </c>
@@ -7593,11 +7125,8 @@
       <c r="F210" s="2">
         <v>2</v>
       </c>
-      <c r="G210" s="2"/>
-      <c r="H210" s="2"/>
-      <c r="I210" s="2"/>
-    </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="211" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A211" s="4" t="s">
         <v>385</v>
       </c>
@@ -7616,11 +7145,8 @@
       <c r="F211" s="2">
         <v>1</v>
       </c>
-      <c r="G211" s="2"/>
-      <c r="H211" s="2"/>
-      <c r="I211" s="2"/>
-    </row>
-    <row r="212" spans="1:9" ht="61" x14ac:dyDescent="0.2">
+    </row>
+    <row r="212" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A212" s="2" t="s">
         <v>642</v>
       </c>
@@ -7639,13 +7165,11 @@
       <c r="F212" s="2">
         <v>2</v>
       </c>
-      <c r="G212" s="2"/>
       <c r="H212" s="2" t="s">
         <v>643</v>
       </c>
-      <c r="I212" s="2"/>
-    </row>
-    <row r="213" spans="1:9" ht="46" x14ac:dyDescent="0.2">
+    </row>
+    <row r="213" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A213" s="2" t="s">
         <v>646</v>
       </c>
@@ -7664,11 +7188,8 @@
       <c r="F213" s="2">
         <v>4</v>
       </c>
-      <c r="G213" s="2"/>
-      <c r="H213" s="2"/>
-      <c r="I213" s="2"/>
-    </row>
-    <row r="214" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="214" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A214" s="2" t="s">
         <v>649</v>
       </c>
@@ -7687,11 +7208,8 @@
       <c r="F214" s="2">
         <v>2</v>
       </c>
-      <c r="G214" s="2"/>
-      <c r="H214" s="2"/>
-      <c r="I214" s="2"/>
-    </row>
-    <row r="215" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="215" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A215" s="4" t="s">
         <v>88</v>
       </c>
@@ -7710,11 +7228,8 @@
       <c r="F215" s="2">
         <v>2</v>
       </c>
-      <c r="G215" s="2"/>
-      <c r="H215" s="2"/>
-      <c r="I215" s="2"/>
-    </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="216" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A216" s="4" t="s">
         <v>502</v>
       </c>
@@ -7733,11 +7248,8 @@
       <c r="F216" s="2">
         <v>1</v>
       </c>
-      <c r="G216" s="2"/>
-      <c r="H216" s="2"/>
-      <c r="I216" s="2"/>
-    </row>
-    <row r="217" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="217" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A217" s="2" t="s">
         <v>654</v>
       </c>
@@ -7756,13 +7268,11 @@
       <c r="F217" s="2">
         <v>2</v>
       </c>
-      <c r="G217" s="2"/>
       <c r="H217" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="I217" s="2"/>
-    </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="218" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A218" s="2" t="s">
         <v>658</v>
       </c>
@@ -7781,11 +7291,8 @@
       <c r="F218" s="2">
         <v>1</v>
       </c>
-      <c r="G218" s="2"/>
-      <c r="H218" s="2"/>
-      <c r="I218" s="2"/>
-    </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="219" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A219" s="2" t="s">
         <v>661</v>
       </c>
@@ -7804,11 +7311,8 @@
       <c r="F219" s="2">
         <v>1</v>
       </c>
-      <c r="G219" s="2"/>
-      <c r="H219" s="2"/>
-      <c r="I219" s="2"/>
-    </row>
-    <row r="220" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="220" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A220" s="4" t="s">
         <v>186</v>
       </c>
@@ -7827,11 +7331,8 @@
       <c r="F220" s="2">
         <v>2</v>
       </c>
-      <c r="G220" s="2"/>
-      <c r="H220" s="2"/>
-      <c r="I220" s="2"/>
-    </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="221" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A221" s="2" t="s">
         <v>666</v>
       </c>
@@ -7850,11 +7351,8 @@
       <c r="F221" s="2">
         <v>1</v>
       </c>
-      <c r="G221" s="2"/>
-      <c r="H221" s="2"/>
-      <c r="I221" s="2"/>
-    </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="222" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A222" s="2" t="s">
         <v>666</v>
       </c>
@@ -7873,11 +7371,8 @@
       <c r="F222" s="2">
         <v>1</v>
       </c>
-      <c r="G222" s="2"/>
-      <c r="H222" s="2"/>
-      <c r="I222" s="2"/>
-    </row>
-    <row r="223" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="223" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A223" s="2" t="s">
         <v>669</v>
       </c>
@@ -7896,11 +7391,8 @@
       <c r="F223" s="2">
         <v>2</v>
       </c>
-      <c r="G223" s="2"/>
-      <c r="H223" s="2"/>
-      <c r="I223" s="2"/>
-    </row>
-    <row r="224" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="224" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A224" s="2" t="s">
         <v>673</v>
       </c>
@@ -7919,11 +7411,8 @@
       <c r="F224" s="2">
         <v>1</v>
       </c>
-      <c r="G224" s="2"/>
-      <c r="H224" s="2"/>
-      <c r="I224" s="2"/>
-    </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="225" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A225" s="2" t="s">
         <v>673</v>
       </c>
@@ -7942,11 +7431,8 @@
       <c r="F225" s="2">
         <v>1</v>
       </c>
-      <c r="G225" s="2"/>
-      <c r="H225" s="2"/>
-      <c r="I225" s="2"/>
-    </row>
-    <row r="226" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="226" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A226" s="4" t="s">
         <v>93</v>
       </c>
@@ -7965,13 +7451,11 @@
       <c r="F226" s="2">
         <v>1</v>
       </c>
-      <c r="G226" s="2"/>
       <c r="H226" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="I226" s="2"/>
-    </row>
-    <row r="227" spans="1:9" ht="31" x14ac:dyDescent="0.2">
+    </row>
+    <row r="227" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A227" s="4" t="s">
         <v>186</v>
       </c>
@@ -7990,11 +7474,8 @@
       <c r="F227" s="2">
         <v>2</v>
       </c>
-      <c r="G227" s="2"/>
-      <c r="H227" s="2"/>
-      <c r="I227" s="2"/>
-    </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="228" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A228" s="2" t="s">
         <v>679</v>
       </c>
@@ -8010,21 +7491,49 @@
       <c r="E228" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="F228" s="2"/>
-      <c r="G228" s="2"/>
-      <c r="H228" s="2"/>
-      <c r="I228" s="2"/>
-    </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A229" s="2"/>
-      <c r="B229" s="2"/>
-      <c r="C229" s="2"/>
-      <c r="D229" s="2"/>
-      <c r="E229" s="2"/>
-      <c r="F229" s="2"/>
-      <c r="G229" s="2"/>
-      <c r="H229" s="2"/>
-      <c r="I229" s="2"/>
+      <c r="F228" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A229" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="D229" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="F229" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A230" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="D230" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="F230" s="2">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>